<commit_message>
Get daily reddit data: Tue Jul 29 08:14:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_03.xlsx
+++ b/data/collected_data/2025_08_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3406 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1mc5hj9</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Neon Pink with Lines</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc5hj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1mc5dte</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>august is approaching...which means apples !! :D</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9yjof9oqrff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1mc59rk</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>My favourite set ever</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc59rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1mc4xmx</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Tried Something Soft and Romantic💅💓</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywmiilb9lrff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1mc4lcz</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Downtown LA nail salon recos?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mc4lcz/downtown_la_nail_salon_recos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1mc45jj</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>My first nail art🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpesfxjicrff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1mc4501</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Remove polish</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mc4501/remove_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1mc3uwu</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Removed gel overlay and found this...</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4r5nt339rff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1mc3q7h</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Just did my totally normal nails.</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc3q7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1mc3owo</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Acrylics into press ons</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mc3owo/acrylics_into_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1mc3ety</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>new set!!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc3ety</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1mc3bg0</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Pink with black flames gel nails I got done for BlackPink’s concert</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc3bg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1mc38vx</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>First time using Gel X press ons</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35nwpidj2rff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1mc2ssz</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My first time getting acrylics! &lt;3</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyk63wcwxqff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1mc2oyw</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>As a fan of cherries, I saw this set and I loved it 😍 I would add more cherries anyway 😂🫶🏼</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ate6lz0vwqff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1mc2ivd</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>These are my natural nails btw</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc2ivd</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1mc1pel</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc1pel</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1mc1gfn</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Galaxy, Oil Spill, or Psychedelic? What Should I Name This?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc1gfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1mc08we</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Recent sets practicing w/ 3D gel and painting designs</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc08we</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1mc055n</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Manicurist green flash with different LED?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mc055n/manicurist_green_flash_with_different_led/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1mc00v4</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Can I use a regular acetone free nail polish remover to remove Manicurist Green Flash nails?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mc00v4/can_i_use_a_regular_acetone_free_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1mbw891</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>🤡 happy/sad clown nails 🤡</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30ybgy94cpff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1mbwumk</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>What can I add to these nails?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbwumk</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1mbxsj1</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Problem with green fungi</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbxsj1/problem_with_green_fungi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1mbzu50</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Shadow &amp; Light 🌗</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ntdb90836qff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1mbz6f2</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>"natural" acrylics</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0r2z24i0qff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1mbz1v1</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Starter nail kit suggestions?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbz1v1/starter_nail_kit_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1mbz0np</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>do we like 😁</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ovobbz5zpff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1mbyyjr</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Unintentionally did Wicked nail colors on myself</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/agpk1azmypff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1mbymlf</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>This beautiful freestyle</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbymlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1mbyf0e</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Builder Gel help!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbyf0e/builder_gel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1mby3da</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Nail strengthing</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mby3da/nail_strengthing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1mby1z2</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>These ended up being my engagement nails!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mby1z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1mbxx0a</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Need birthday nail suggestions</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7sdnbbnuppff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1mbxs15</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Summer flowers by me💐🦋</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbxs15</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1mbxprn</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Dented nails?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbxprn</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1mbxp19</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Private nail tech for the win!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szgfj881opff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1mbw6c0</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>gelx help</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbw6c0/gelx_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1mbw1t9</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>cheapest high quality e-files?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbw1t9/cheapest_high_quality_efiles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1mbvyd4</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>How I started...and one year later. Im pleased. I can't wait to see what another year does for my painting.</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbvyd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1mbvrwe</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Gel X Questions</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbvrwe/gel_x_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1mbvoxr</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>took me 5 hours but i am so proud this is my 6th set ive done so far 💚💚💚</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbvoxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1mbvjlq</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Third natural nail attempt</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbvjlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1mbvjih</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Trying to take care of my hands better as a guy :) what’re some of your favorite “hand and nail hacks”?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8450bgr6pff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1mbssig</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>HELP!!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbssig</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1mbtaqn</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Too much cuticle removed? What am I looking at?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbtaqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1mbs21q</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a good polish for my wedding?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbs21q/can_anyone_recommend_a_good_polish_for_my_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1mbqhdi</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Press on nails come off in the shower</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbqhdi/press_on_nails_come_off_in_the_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1mbqpkb</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Pedicures- how to ask for what I want?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbqpkb/pedicures_how_to_ask_for_what_i_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1mbo6ex</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Can I use regular Nail glue on Gel tips? Or what do I buy?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u1w66tlrnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1mbpuma</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Opal Inspired 🥰</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5dxcdom2off1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1mbv7gc</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>First at home set!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbv7gc</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1mbublj</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Cute!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3o3mk5ixoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1mbu5fw</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Sweet summer nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbu5fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1mbu4t7</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Dip Nail Set</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oy703b44woff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1mbu0r5</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Summer nails 💅</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2idsyaavoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1mbu0qd</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Mixing red nail polish with clear</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbu0qd/mixing_red_nail_polish_with_clear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1mbtq2z</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Summer abstract</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea7zh8k6toff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1mbtp2y</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>First Time Getting Builder Gel Nails. How Do They Look?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbtp2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1mbtgr6</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Usan el efecto Cat eyes?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbtgr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1mbtggm</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My nails, by me.</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t91o9n8roff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1mbt95y</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>New nails 💕💕</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v84r86aupoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1mbt47c</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Seeking Pearl Nail Product Recommendations for My Wedding (Not DIY – Will Bring to Pro Tech)</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbt47c</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1mbt312</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Planning my next set. What do you think?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i3mv3p7mooff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1mbsojp</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>dupe for this shade??</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czjdilksloff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1mbrxz4</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Post hard gel</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbrxz4/post_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1mbr7cz</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>my vacation nails</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbr7cz</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1mbqigb</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Super Light Baby Blue 💙</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1lxipt47off1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1mbqhcl</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>How to make press ons look better on?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5ngdi7x6off1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1mbq3cj</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Nail stickers on natural nails</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbq3cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1mbpeln</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Russian Manicure Safety Question</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbpeln/russian_manicure_safety_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1mbpkyd</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>I feel like they are my favorite nails ever I swear</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysxxg71u0off1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1mbpkud</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>New Set!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbpkud</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1mbktfi</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Is this a ring of fire?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9xirtar5nff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1mbmmyr</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>admiring the shifts 💕</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbmmyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1mbp9au</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>First time EVER doing nails. Took 6hrs 💀</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unufcyjoynff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1mbp1xj</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Don't sleep on drugstore polishes, this might just be my new fav!! Revlon "Daydreamer"</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zy8ubw4cxnff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1mboyyw</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>How to handle breakage?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60mwto5uwnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1mbo637</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>KBShimmer - Best Witches</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbo637</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1mbnmfp</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Chrome nails infill?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doi4rnwynnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1mbncd2</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbncd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1mbnarc</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>A nightmare</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbnarc</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1mbnacs</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Charged for Fixing nail due to product issues</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbnacs/charged_for_fixing_nail_due_to_product_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1mbn5zd</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>in love</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbn5zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1mblzci</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I wanted to go for a faded pink, $55 for it</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4twcg29dnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1mblrch</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mblrch</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1mblqxm</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Finally got these foils right!!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvyp46wtbnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1mbkngu</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Color name please help!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no2y8u0o4nff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1mbkj7l</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>I made green fluorite crystal nails</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbkj7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1mbkc4y</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Postpartum nails</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kudvg4f62nff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1mbk0fu</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Engagement nails help!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbk0fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1mbiiml</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Why do my acrylics look like this?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbiiml</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1mbi3zx</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>How to remove acrylic nails with nail form method (no tips)</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbi3zx/how_to_remove_acrylic_nails_with_nail_form_method/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1mbazfo</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>My nail tech of two years, now doing a poor job.</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbazfo/my_nail_tech_of_two_years_now_doing_a_poor_job/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1mbc54f</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>What is this nail file called and how can I find it?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mbc54f/what_is_this_nail_file_called_and_how_can_i_find/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1mbf1qw</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>My version of rainbow nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbf1qw</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1mbewgd</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>How to fix stained nails</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuy60ga10mff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1mbjehk</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Couldn’t decide which design to do, lol…</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbjehk</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1mbix33</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>these were my birthday nails</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbix33</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1mbgqwi</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Found cat stickers at the nail supply store</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbgqwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1mc4eqd</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Kinda spacey!🫢</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc4eqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1mc46av</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>My first nail art🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpesfxjicrff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1mc31xr</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Oddities ✨</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e0n86yrg0rff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1mc31xa</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>a summer of chrome</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc31xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1mc24c5</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>ILNP - Glowstick, velvetized ✨</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc24c5</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1mc23zv</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Dupe Request: Blackheart Nail Polish in Moonbeam</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xe1azmzqqff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1mc0wgo</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Swatched up</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8drjldxofqff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1mc0pgj</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Summer temps</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9uxm838ydqff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1mbzjr9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Deep Space so beautiful</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rh1j9imk3qff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1mbzf7l</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Is this just dehydration from acetone or something else?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbzf7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1mbz01s</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Chrome powder on regular nail polish in the wild</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5x78wse0zpff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1mbypbm</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Sweet &amp; Sour Lacquer Spotlight</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbypbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1mby22d</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>2 in 1 blurring base</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mby22d/2_in_1_blurring_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1mby0k3</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Tell me your favorite reflective glitters!!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mby0k3/tell_me_your_favorite_reflective_glitters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1mby0i0</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Looking for recommendations for a scattered holo topper with bigger glitters!</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mby0i0/looking_for_recommendations_for_a_scattered_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1mbxvcb</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Beachy nails!</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbxvcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1mbxq0r</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Comparison Lurid I grieve you everytime I remember to Cracked Wowwww ?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbxq0r/comparison_lurid_i_grieve_you_everytime_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1mbxov3</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Monarch Lacquer Truth or Dare</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbxov3</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1mbxdhk</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>ISO Swatches of Sheer Tint Yellow by Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbxdhk/iso_swatches_of_sheer_tint_yellow_by_emily_de/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1mbx52e</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>I’m sorry, DJ What? Why??</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahbipvzfjpff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1mbwt0q</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>how can i fix the shape of my nail?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbwt0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1mbwpyl</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Dopamine in the Home Depot Parking Lot feat. Lavender Haze</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hpjfg5mzfpff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1mbw5f9</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Anyone recognize these Color Club polishes?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbw5f9</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1mbw3gw</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Summer in a bottle</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbw3gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1mbvxla</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Keeping Cool in the Pool</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbvxla</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1mbvm5h</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Revlon mini haul</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbvm5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1mbvh6v</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Holo Taco Unicorn No. 1 vs. Sassy Sauce Cock a Doodle Doom vs. Sassy Sauce Glampire 2.0</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbvh6v/holo_taco_unicorn_no_1_vs_sassy_sauce_cock_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1mbu7co</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Please help me find this color!</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev3avzpmwoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1mbu0la</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>July Mani Review</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbu0la</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1mbtuvn</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>I will be your undoing...</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u1qlajrztoff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1mbtk67</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at my nails! I’ve always loved crackle!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbtk67</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1mbthr0</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>KB Shimmer Feelin Groovy</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbthr0/kb_shimmer_feelin_groovy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1mbtbak</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Hard gel vs gel</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbtbak/hard_gel_vs_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1mbt75m</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Shimmery dark blue!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbt75m</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1mbstir</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>blank beauty</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfgpv2uqmoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1mbsbqk</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Wasn’t sure how I felt about this polish when I put it on, then I went outside and omg the shift is insane!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/juztqkjajoff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1mbrf4n</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>July PPU arrived!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbrf4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1mbr311</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>A Little Summer Sherbet Ombre Experiment.</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcye83rzaoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1mbr2gk</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>I love adding a sheer to tone up the base!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbr2gk</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1mbqc9i</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Sea Glass</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7lmewfy5off1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1mbqb6l</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Seeking ILNP polishes with the same finish as Sunburst</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbqb6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1mbqb2e</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Clionadh release!</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzrvs0rq5off1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1mbq9lt</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Looking for an Eggplant Jelly</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbq9lt/looking_for_an_eggplant_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1mbq7uo</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Mahalo For 10 Years - Hula Moon</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbq7uo</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1mbpx95</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Casa De Heaven is that OTHER girl</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il9qpft33off1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1mbp7jn</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>How to stop getting this annoying ledge!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbp7jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1mbp2l8</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Fish Fear Daisy Chain Polish</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbp2l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1mbowpu</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Please recommend me a SIGNATURE brownish-red from Essie/OPI (caption)</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v8t6tefwnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1mbogog</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Why do my nails do this when they contact water?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbogog</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1mbo6o1</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>KBShimmer - Best Witches</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbo6o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1mbmyq5</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>What I wore in July 🎆</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbmyq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1mblk19</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Pastel Pink</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mblk19</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1mbl6v7</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Sofa gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbrw1fl88nff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1mbl048</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 has changed the game for me! 3 weeks of growth with no chipping, peeling, or tip wear!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbl048</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1mbkuta</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Lake Day Mani 🫧</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbkuta</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1mbk5sq</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Swatched and organized everything and I am so pleased.</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cppqxech1nff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1mbjmp2</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Is it just me...</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oqwm19t0ymff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1mbjkny</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>First gellac application</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7st3e3rnxmff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1mbjhpe</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>That magical fuchsia flash 💜💥</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7pvuwf73xmff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1mbj6fn</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>July Mani Compilation</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbj6fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1mbih8x</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Got a Chance to Try the Glass Bead Affect</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/31oubwqmpmff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1mbi2fd</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>All my July manis</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbi2fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1mbhrsa</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Rothko inspired nail art</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s38co8hblmff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1mbh211</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Let’s talk base coats</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbh211/lets_talk_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1mbgglw</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>A 3D Printed Magnet Design That Anyone Can Assemble</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qqw1dd85cmff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1mbfnsj</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Brushed steel &amp; undercover neon</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbfnsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1mbfjt9</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Lion's Mane</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbfjt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1mbfeyd</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Flower child Inside/Outside</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbfeyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1mbfd1x</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Nothing like a deep burgundy💃</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbfd1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1mbf5cq</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Can I put a Laquer polish on top of a gel coat?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbf5cq/can_i_put_a_laquer_polish_on_top_of_a_gel_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1mbd7oh</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Don't usually wear sheers but look at the GLOW</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbd7oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1mbcdh1</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Safe Gel X removal for onycholysis underneath?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbcdh1/safe_gel_x_removal_for_onycholysis_underneath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1mbc4sx</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbc4sx/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1mban4r</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Keeping track in 2025</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mban4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1mbak7a</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Name this polish 🧡</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbak7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1mbahvc</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>I love this polish but...</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbahvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1mc5dcf</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>apples :3</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8frura7jqrff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1mc1m3l</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Experimenting with isolated chrome</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l87t2h69mqff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1mc1eho</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Oil Spill or Shroom Trip? Can’t Decide What to Call This One 🌌🫧</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc1eho</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1mc0zcc</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Studio Ghibli GelX</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc0zcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1mbztbj</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>third set!! progress??</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbztbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1mbzqy0</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Shadow &amp; Light 🌗</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b3725hxa5qff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1mbxga3</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>My clients vacation set ✨💜</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptziet30mpff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1mbw8o3</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>First attempt at more complicated nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wsafjc7cpff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1mbvz83</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Blackpink nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0u51kh4apff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1mbuogj</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Fresh set with messy lines</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbuogj</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1mbug3p</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>simple chrome and ombré nails</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs1av57gyoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1mbufdy</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>cherry polka dot nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6rd06gayoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1mbr0f1</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Birthday trip set</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlocc67iaoff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1mbqsid</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>At Home Nail Art Class Day 2 ✨</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbqsid</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1mboi8p</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Tropical. Extra. And just a lil’ too hot to handle 💖🔥</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akztjw3ttnff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1mbkobs</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Green fluorite nails</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbkobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1mbk7g7</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Gel set I did two weeks ago</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbk7g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1mbjtpv</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Ferris Wheel Silhouette featuring the queen of my house. Just a simple little something in my cityscape set.</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hzi8okq1zmff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1mbjgug</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7eqrqh2ywmff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1mbjggb</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>a little camo print and chrome moment.</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbjggb</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1mbgjfx</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>🧡</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbgjfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1mbfx51</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Anyone able to design a nail based on villanelle’s blazer pattern?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nznlf7f18mff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1mbft7q</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>i love this fake piercing trend 😍</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwaucwpc7mff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1mbe0bq</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>New nails 💅🏻 💕</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv7nrhv7slff1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 30 08:14:19 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_03.xlsx
+++ b/data/collected_data/2025_08_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C501"/>
+  <dimension ref="A1:C727"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8950,6 +8950,3848 @@
         </is>
       </c>
     </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1md038x</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>I know they're simple, but I love them!</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34yqjzvkqyff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1mczv1u</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>New Set!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mczv1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1mczldy</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Loving floral nails 🌸🩵</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2c93z0zkyff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1mcz6j3</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Cherry tulips</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcz6j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1mcwov6</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>HELP - uncured gel on acrylic</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlhe09asqxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1mcycn2</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Hi my first time here. My new manicure</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cuzfwuc7yff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1mcxvtu</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Anything i could do better on?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qeptv6gg2yff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1mcxuvf</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Nightmare fuel</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j02esvc72yff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1mcxngw</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>I love you, you are next ❤️😍✨🤩</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08lg1ci50yff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1mcwa34</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Likely my last summer set for the year, made it extra fun!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcwa34</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1mco8pw</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Inspired by sleeping beauty</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79zszthitvff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1mcq05q</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>What do I ask for if I just want a polish change, light nail shaping and cuticles managed on my feet? I would like to be succinct and use the right lingo to help bridge a potential language gap.</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcq05q/what_do_i_ask_for_if_i_just_want_a_polish_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1mcruig</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Why do my nails have this texture a day or two after doing them?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc82rgsxkwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1mcw07p</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Does anyone else have a perfect nail and a nightmare nail or is that just me?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4kke7nekxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1mcvzus</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Gel manicure bleached out</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcvzus/gel_manicure_bleached_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1mcvvxr</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Very strong without broken</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1o0996rbjxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1mcnkt5</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Did anyone here develop a gel allergy and have issues with contacts after?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcnkt5/did_anyone_here_develop_a_gel_allergy_and_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1mcquz1</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Base Coat</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcquz1/base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1mcr9of</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>does anyone else's nails grow like this</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/161ayhu8gwff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1mcs7w7</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Too soon?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcs7w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1mcv96p</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Troubleshooting gaps between natural nail and press ons?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcv96p</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1mcuxek</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I suck at hand poses</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcuxek</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1mcvdrl</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Are these too long? They're for engagement pics...</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bi16qvuexff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1mcvcne</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>did my cousins nails</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcvcne</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1mcv0jk</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>I painted a cute little cow abduction nail, just for fun.😜🛸🐄</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hf2nc2inbxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1mcuv1y</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Non-binary guy here. I started caring for my nails back in January, but have really dialed in to my routine the last couple of months. I’m looking for slightly androgynous, but mostly clean. Happy with my current progress! (Before on last slide)</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcuv1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1mcuv1p</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>summer nails</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcuv1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1mcuu0c</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiqdclp1axff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1mcs8ri</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Gel Beetles Top coat crapped out after 2 years…I didn’t have any other top coat, how do I save this with my new one coming in tomorrow</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7om12z8owff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1mcsqrb</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Maybelline- glowing glimmer</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcsqrb</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1mcts8f</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Bruise or bacteria?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcts8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1mctzc5</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>I need your opinion on DND and other good brands🙏</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mctzc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1mcuc6g</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Are gel x supposed to be this thick underneath?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcuc6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1mcubug</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Beachy Sets 🐚</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcubug</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1mcuagm</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Unsure about solo design color.</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q63kyquh5xff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1mctyuj</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Loving my new cat eyes!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6ax27ss2xff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1mctow0</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Estás uñas para una quinceañera 💅</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mctow0</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1mctkih</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Pretty in Pink! 💖</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mctkih</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1mct9sw</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Is The Gel Nail Polish I’m Using, Safe?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mct9sw/is_the_gel_nail_polish_im_using_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1mcrrcf</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Getting into that Halloween Mood 😁</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcrrcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1mcri7c</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcri7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1mcra5z</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>very milky peachy pink</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcra5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1mcr67y</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Got my nailed filled for the first time!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcr67y</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1mcr14f</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>The next one will be with violet tones</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvkpkz3cewff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1mcr089</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>my boyfriend took this pic for me.. the tiny feet are killing me lol</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fihcuia5ewff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1mcqmrf</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Lemonade 🍋</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t3pdig9bwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1mcq6sv</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Gel nails burnt hair smell</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcq6sv/gel_nails_burnt_hair_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1mcq3qk</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Relate? 🤣</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g74hco587wff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1mcpavs</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Summer Flowers</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o3lvuvr41wff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1mcp8ee</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Hello Everybody! Today I have done my very first gel nails 💅 Please let me know what you think and where I can improve 🙏🏻 🙂</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcp8ee</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1mcp7ji</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>First time doing my own gel nails!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxuzm73h0wff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1mcp1ak</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Purple marble with gold foil</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcp1ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1mcowvx</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>New Design (Monochromatic French Tips with Cat Eye Polish)</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjuduuqcyvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1mcowvp</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Cloudy pink nails with complementary cat pics</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcowvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1mcoosl</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>I love blooming gel</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tnnjvynwvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1mcoeer</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>first korean gel manicure</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcoeer</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1mcob85</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Pearl tides 🐚</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8ibl5wztvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1mco2wz</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Improvised and dissociative nail art that I kinda like 💅🏼😂☁️🌿</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mco2wz</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1mco2vn</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Why do these look odd to me?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mco2vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1mcnw35</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Gel x, acrylic, press ons don’t last</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcnw35/gel_x_acrylic_press_ons_dont_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1mcmzed</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>What is causing the color change?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcmzed</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1mcmds5</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I made a rose quartz press on set for my mom</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e793molpgvff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1mcm5k1</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>It’s so hard to do claws, but it’s always worth it. What do you think of my new rainbow claw design? 🦋🩵</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stm9my26fvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1mcheqp</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Do Rubber Bases Actually Work For Brittle Nails?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wi1tjutqjuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1mclvk7</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>What nail shape would suit me?!!!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjxmx1ebdvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1mclt1r</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Polka Hearts</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aamv0swucvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1mclpll</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Advice on transitioning from liquid gel nails?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mclpll/advice_on_transitioning_from_liquid_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1mcloqs</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Junk nails I did that remind me of iSpy and Lisa Frank</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcloqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1mclmve</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Some white chrome nails</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/th4lwndpbvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1mclhq1</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>getting chrome acrylic extensions for the first time!inspo pic from pinterest, and the pinterest post gives credit to @salonulu_</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3957toqavff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1mclec6</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Feeling pretty in pink 💕</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb16z7z2avff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1mcka95</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>this set was inspired by x-rays 🩻</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcka95</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1mck1ic</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mck1ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1mcl3ks</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Looking for honest opinions about which nail shape looks best on my hands!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcl3ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1mcl0go</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>My favourite set I've ever done, ladies and gents</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcl0go</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1mckkol</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Cat acrylic nails in Albany NY?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mckkol/cat_acrylic_nails_in_albany_ny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1mckjap</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Builder nail tips: any and all! They’re thick right now.</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mckjap</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1mckiv8</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Builder nail tips: any and all! They’re thick right now.</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mckiv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1mck4rh</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>My first week of doing nails!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mck4rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1mcjtjr</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>I Fell I love with a KI Design, is it possible?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u12tz25kzuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1mcivdm</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Please help me decide which nail shape looks best on my hands</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcivdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1mcjq4v</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>I got these done exactly 1 month ago for my wedding. The retention!! 👏👏</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuqpghnwyuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1mcjaz1</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Do you guys know an app in which I can elaborate my nails before doing it?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcjaz1/do_you_guys_know_an_app_in_which_i_can_elaborate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1mciyvu</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Is it possible to remove acrylics and/or dip nails in a way to be able to use them as press-ons later?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mciyvu/is_it_possible_to_remove_acrylics_andor_dip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1mcim03</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Is it ok to get a new full set of acrylics  every time instead of doing fills</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mcim03/is_it_ok_to_get_a_new_full_set_of_acrylics_every/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1mcifpr</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>How can I improve my weak nails? And what color would look good on me??🥺🥲</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru93k0lequff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1mci92n</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Don't hate them but don't love them either</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0f4abv6puff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1mci8h8</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>My birthday set 🔮🌙✨</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mci8h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1mci6uo</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Do you file off your builder gel when you do a new set or just file off the shiny part of your nail design?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mci6uo/do_you_file_off_your_builder_gel_when_you_do_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1mchixx</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Script Tattoo Nails 🖋️</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mchixx</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1mchkqm</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>second set I did</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecu4bk9tkuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1mchioa</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Fish</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mchioa</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1mchdb3</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Mermaidy paper forms 🧜‍♂️</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mchdb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1mchbby</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Best Gel-X Supplies</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mchbby/best_gelx_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1mchang</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Ideassss??🥹</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6jcgee0juff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1mch3qg</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>stained nails help!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnt52kzrhuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1mch9dz</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Broken nail with gel</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35zl59gsiuff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1mch67o</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Nails in healing era 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yi5r3d8iuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1mc3wjc</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>What do I do when the builder have loosened in the edges?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmtrhxan9rff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1mc46ln</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Nails art</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc46ln</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1mcywtm</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Nail bed massacre</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcywtm</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1mcynop</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>ISO a polish that matches Saturn's south polar vortex</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3jcashnayff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1mcylc3</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>weird unevenness on magnetic polish??</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4sblevfx9yff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1mcwqug</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Trial run with blue to match a dress I’m wearing this weekend 💙🥶🦋🐳</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ced7f2darxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1mcwc81</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Similar formula to Cirque but better reds?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcwc81/similar_formula_to_cirque_but_better_reds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1mcw7xv</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Question for techs: men coming to a salon</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcw7xv/question_for_techs_men_coming_to_a_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1mcw5lb</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>My husband asked me to paint his nails for his upcoming game convention</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/erib13prlxff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1mcvi7i</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Why do I not like it?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcvi7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1mcvcl0</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>freehand french people— how do yall do it?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcvcl0/freehand_french_people_how_do_yall_do_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1mcv80c</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>If a thermal polish had to die…</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcv80c</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1mcuvaf</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>What polish is everyone looking to buy for the upcoming month’s ppu? 😊</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcuvaf/what_polish_is_everyone_looking_to_buy_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1mcunqo</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>My favorite pink 🩷</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcunqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1mcu514</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Doth my eyes decieve me?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcu514</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1mctzcz</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Pre-, mid-, and post-chop</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mctzcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1mcty3p</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Sidekick</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12jeagzm2xff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1mcssim</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>How to save endlessly delaminating nails? Can fake nails help?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcssim/how_to_save_endlessly_delaminating_nails_can_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1mcsrue</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Magnetic fail</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eh49xpspswff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1mcsnvo</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>We need something like this to paint easily while the magnet is actively spinning</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2uartmsrwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1mcsm64</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>First BKL haul</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcsm64</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1mcsicq</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Help a surgery girly out!</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcsicq/help_a_surgery_girly_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1mcs0uz</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Had this for a while but never used it! I'm in love ❤️</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj2ir09fmwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1mcrxq2</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Taking blood pressure causing nails to split</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1u7geiolwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1mcrbjk</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>lurid prototype 254 should become a permanent shade!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkbh1rzngwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1mcr9jg</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>PPU Delivery Day 😍</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/34ckqy91gwff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1mcr6d9</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>It's PPU ***AND*** DD delivery day!</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcr6d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1mcqu6q</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Base Coats</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcqu6q/base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1mcqllu</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Nude/pink base color for nail art?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcqllu/nudepink_base_color_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1mcqfbc</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>What is this design called &amp; any tips?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjphmw2o9wff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1mcqc8v</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>i was in need of some bling so i pulled out the Holo Tacos 💿🌮</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcqc8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1mcq95e</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Starry nails 💫</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5zd2799d8wff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1mcq2co</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Uno Mas Colors - La Llorona (indoors, outdoors, in the dark!)</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcq2co</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1mcpxeu</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Did anyone here develop a gel allergy and have issues with contacts after?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcpxeu/did_anyone_here_develop_a_gel_allergy_and_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1mcpfyi</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Duel of the Doomicorns: Comparison of the Original vs 2.0</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcpfyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1mcp98l</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>too good not to share ✨</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcp98l</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1mcor4w</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Another surprising finish</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m378rbj6xvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1mcojvl</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>2 hauls in one day!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcojvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1mcoixl</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>My nail girl ate with these</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcoixl</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1mcodia</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Good nude colors for super Pale and cool toned people?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1vvj2bguvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1mco1d0</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Cadillacquer Reflections, Glass Bead Edition</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y83wcuf2svff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1mcnnt1</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Help top coat drying too fast</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcnnt1/help_top_coat_drying_too_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1mcnld1</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Riptide🌊</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcnld1</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1mcnghg</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Mooncat House of Hades Vs Sinful Colors Blue by you</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcnghg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1mcndpa</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Blueberry nails w/ stickers</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hi6gv7hnvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1mcmjry</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>It's amazing what you can do with a creme ✨</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flytiblbhvff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1mcmhiz</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>nails curving inwards at the sidewalls?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcmhiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1mcm9jg</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Glowy and Shifty</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcm9jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1mcltfw</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Help ID or dupe?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcltfw/help_id_or_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1mckxoc</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>First PPU Order</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1mqg2lux6vff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1mclhg3</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Magnet safety?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mclhg3/magnet_safety/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1mclgbu</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers Stiff as a Board</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mclgbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1mclc8i</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Summer Shiny</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgpcd77o9vff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1mcl9wa</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Neon green skittle 💚💚💚</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcl9wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1mckbr9</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>OPI's "What's Your Mani-tude?" 2025 Fall Collection</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mckbr9/opis_whats_your_manitude_2025_fall_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1mck7dp</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Mooncat 404 Soul Not Found and Port 6666 Dupes???</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mck7dp/mooncat_404_soul_not_found_and_port_6666_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1mck0lh</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Quite Literally Dead Inside :: Polished for Days</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcjkmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1mcjzmg</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Rum Ham</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcjzmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1mcjj34</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Favorite Top Coat/Speed Dry?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcjj34/favorite_top_coatspeed_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1mcj2qb</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>glitter in jelly bases my beloved</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcj2qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1mcj1u3</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Roundup of everything I wore in July</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcj1u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1mciehd</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>2025 Rewind Haul</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/irbl7af6quff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1mci9bp</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Merkitten sibling?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l52gk8k8puff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1mchv1i</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>strawberry nails ✨</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mchv1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1mchtxt</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Okay….this is new</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kmyuk6lemuff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1mchox3</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Polished for Days - Snow Cap</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mchox3</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1mcgvfl</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Hairline crack in builder gel</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkmditwbguff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1mcgssd</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>A pastel experiment in jellies + magnetic topper</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hobzfotrfuff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1mcgsnn</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Reddit Laquerists Discord Anniversary Customs</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpl45tjtfuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1mcgry6</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>I 💜 Flip Side</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bfiwo0lofuff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1mcgcsr</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I (don't) think I've had enough (swatches) of this polish</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwy68huxcuff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1mcfhja</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>I don't need this polish because I already have one just like it, but I still want it because I am absolutely dying over the name</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyu2vp877uff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1mcf3oa</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>My favorite polish from my first ever PPU purchase</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcf3oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1mcekf7</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Baja Blast Nails (without Baja Blasted polish)</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcekf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1mcech8</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Nail polish that is similar to tigers eye?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcech8/nail_polish_that_is_similar_to_tigers_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1mce8d3</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Looking for color match recs for my latest project</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mce8d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1mcdl8t</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Bluebell 💙💙</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcdl8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1mcdf9b</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>What is the dl on "peely bases"???</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mcdf9b/what_is_the_dl_on_peely_bases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1mcd6ui</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Help me pick my birthday nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcd6ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1mcd578</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>PPU from the top of a mountain 🌄</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcd578</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1mccsx6</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Bog Dweller + Spinning 🧲 + Chrome Powder</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/25nasauuotff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1mccs3q</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>How to fix stained nails</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joqignopotff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1mccqm4</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Pelvic Sorcery is magical</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r3sxo9gaotff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1mccp74</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>TFW you completely forgot you ordered more polish...</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mccp74/tfw_you_completely_forgot_you_ordered_more_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1mccm66</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Could Cirque Colors Pitaya achieve this look?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl1yza1kntff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1mccf3i</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>my sour apple rings order is missing thanks to USPS. what would you do?!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mccf3i/my_sour_apple_rings_order_is_missing_thanks_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1mccc54</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Barista Bundle ☕️🤎</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcca0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1mcc7pz</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Concert nails for Linkin Park concert! Based on Chester’s tattoos</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss0a5hop9tff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1mcc0r7</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>cock-a-doodle DOOM 💜</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7yoonkubjtff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1mbw9lh</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Can anyone help me grow my damaged nails back?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaoitz5wbpff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1mbvv9g</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Best Flakie Brand</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mbvv9g/best_flakie_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1mbrwwm</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Have suddenly developed a gel allergy</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbrwwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1mcav9x</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Delayed brat summer</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy87fd2latff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1mcamxh</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Still learning</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddzz57js8tff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1mcaltd</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>First attempt at stamping. It's bad, but I think I'll get better at it</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/980c4j2k8tff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1mcalp2</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Car Nails Ready DO Hit Different...</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/91g7gzqh8tff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1mcaenn</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>so bright! so loud! 💥</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g27gmdqy6tff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1mcadkp</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Swatched &amp; labelled my whole collection</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcadkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1mc9sla</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Why does my nail polish peel off?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mc9sla/why_does_my_nail_polish_peel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1mc9rro</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>💛💚Neon Gradient🩵💙</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc9rro</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1mc8fva</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Nails never dry properly 😭</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0ymlnj9psff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1mc8cgc</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Ignore the summertime sweater hands</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc8cgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1mczn7c</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Design of the day, I love doing my clients' nails 🤭</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrm2fkzjlyff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1mcyro9</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>From 1 to 10, how much do they give you?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7urmhnwvbyff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1mcv9uc</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>❤️❤️</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcv9uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1mcy1uu</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Amber wearing armor</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1ljuyjg2yff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1mcwm73</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>My take on the birth of Venus</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/51dfwkj3qxff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1mcw159</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Holographic Nails Breakdown ✨</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfbmeqkmkxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1mcuzda</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>I painted a cute little cow abduction nail, just for fun.😜🛸🐄</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzd5xd8dbxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1mcuwpm</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Who to vote for the cat effect?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qczdxk6paxff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1mcuvmk</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Do you like snake charm?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cawzr4sfaxff1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1mcse79</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Someone tell me if they are pretty?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edu3e7hjpwff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1mcs9tg</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Too soon?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mcs9tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1mcqkrm</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>How to improve these press-on nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6at33euawff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1mcpbi1</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Summer Flower Nails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jyyjuj591wff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1mclt8n</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Junk nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mclt8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1mckc3b</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>final versión of this set inspired by x-rays 🩻</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18839bgx2vff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1mcjr08</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Red/black nails ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73ixj9w2zuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1mcjn22</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Happy National Chicken Wings Day 🐥</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7rwvl5cyuff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1mcfptc</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Howl's Moving Castle mani for GenCon</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddtoaacp8uff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1mcfejo</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Dollar tree stamp plate</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dohq4len6uff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1mcef2m</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>fav set I did recently 😻</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ejvmov00uff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1mccc97</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Un poco de color por aquí !!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mccc97</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1mcbcaq</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>A Little Aura Gel X</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khr098v7etff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1mc9frh</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>My polish changed color?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ccf3qhtysff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1mc8u8k</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>But what about us neurospicies?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mc8u8k/but_what_about_us_neurospicies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1mbw918</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>A nice way to combine colors and designs</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mbw918</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1mc7pjm</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Did my friend's nails for the first time</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mc7pjm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 31 08:14:42 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_03.xlsx
+++ b/data/collected_data/2025_08_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C727"/>
+  <dimension ref="A1:C915"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12792,6 +12792,3202 @@
         </is>
       </c>
     </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1mdvrk7</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>This was my first time trying press on nails. Is it super noticeable that they are press ons? How can I make them look better?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdvrk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1mdvr2b</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Anyone got a referral code for Pure Nails /Halo?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mdvr2b/anyone_got_a_referral_code_for_pure_nails_halo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1mdvlh0</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Ombré Nude🧡</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdvlh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1mdvg37</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I give them 2 weeks</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdvg37</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1mdvb1d</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>In love with my new set!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jusllh3qy5gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1mdtqdz</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Polish Search</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63m6kcaxg5gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1mduuqr</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Brillan en la oscuridad! Hasta el momento las mejores uñas que me hice.</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mduuqr/brillan_en_la_oscuridad_hasta_el_momento_las/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1mdule9</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Rough draft of...</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw48p80fq5gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1mdu3oh</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>did these myself with actual proper equipment for the first time, so happy with the results 💞</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/192dr25vk5gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1mdtm5j</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Vampy nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/93toequof5gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1mdthf7</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Wedding Nails Thoughts?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdthf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1mdswhj</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Nail polish recs for my collection?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppmq722785gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1mdstw2</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>mani again after too long</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdstw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1mdqlpm</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Woke up one day and decided I wanted to get creative and learn how to do nails</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdqlpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1mdq7nu</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>on vacation and had to get my nails done</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26vxnngji4gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1mdpzdf</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Duck Nails 🌸🐤</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdpzdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1mdpvt6</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>First time trying this shape 💛</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdpvt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1mdp6tf</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>are my nails cute?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdp6tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1mdp7wj</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>my nail tech KILLS everytime</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdp7wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1mdpnxe</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>That Fuzzy Texture Hits Different - Loving the Texture Contrast on This Set</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdpnxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1mdpmpz</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Simple and cute</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3hdjolod4gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1mdp2cs</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>✨✨✨✨</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdp2cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1mdow0y</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Had a lot of fun just following the vibes on this set</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fx6j4cf74gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1mdoc6f</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>finally tried polka dots!!!</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdoc6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1mdo74b</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Who's That Pokémon?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdo74b</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1mdo32l</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Broken nail 😭 help!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdo32l</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1mdnxm3</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Cat eye 💙🩵✨😍</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dquo0y8z3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1mdmawx</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Damage from gel?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mdmawx/damage_from_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1mdndkg</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Set I did on myself today</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdndkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1mdmypm</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izex54u3r3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1mdmktp</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Practicing application &amp; designs.🫶🏼</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdmktp</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1mdm9od</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Delicious 🍒</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdm9od</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1mdm74j</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Rhinestone frenchies</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdm74j</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1mdm49x</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>The nails vs the inspo pic 🤪</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdm49x</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1mdkzh9</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Black dot on gel</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdkzh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1mdjuj8</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Love island inspired nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82bbd3n833gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1mdl83j</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Are these considered long</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdl83j</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1mdl6lz</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>my fav set !</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia9h9il3d3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1mdl51h</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>First time doing my own nails!!</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6g0cc9rc3gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1mdl39j</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>How to successfully use press on nails?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mdl39j/how_to_successfully_use_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1mdkz3e</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>natural nails but better</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2g7kuyhb3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1mdkfht</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>What do you think of these?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdkfht</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1mdk9xc</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Press On Nail Novice</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdk9xc</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1mdk4zl</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>MoMA/Met nails!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4w5zn5c53gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1mdjw36</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Pingu nails for a client! - done by me and hand-painted…it’s giving SlipNOOT</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdjw36</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1mdj0fx</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>First Time Acrylics. Am I critical?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdj0fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1mdjj8b</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>First time getting my nails done 🥰</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s28vrw0u03gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1mdj1ei</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>What decent brands have the best sheer/jelly nude/nude pink collections.. I swear if they are out there, I can’t find them lol</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdj1ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1mdipkw</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Reverse teeth nails I made 🦷🖤</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xig62xr2v2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1mdijlr</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>they’re done ✨</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/roy7aoqut2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1mdibbo</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>What is a similar product?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9cmfux9s2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1mdi9e5</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Wedding Nail Fail?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdi9e5</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1mdi52k</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>First time getting dip</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylvp0ng1r2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1mdi467</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7suvkasvq2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1mdhz0c</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Black and red ombré</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25gg6cjvp2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1mdgyf6</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Went to my artist with “Italian Summer” she said Say Less!!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdgyf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1mdhweh</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Love my new set! (3 week fill cuz I *somehow* broke a nail?? First time ever)</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utp6uua6p2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1mdhcm8</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Idk if I like the look</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdhcm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1mdhckq</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Love my cowgirl nails. 🐮 👢 🐎</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcet5brjl2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1mdh0v2</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Milky White Beetles is gorgeous!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utvlcgq9j2gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1mdgh81</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>First time making press ons! ٩(๑❛ᴗ❛๑)۶</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdgh81</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1mdf5kd</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Press-ons from Temu</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdf5kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1mdf3rj</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>New Set 🫧🤍</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpgoxbf562gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1mdf3n1</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>5 week nails😟</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1qg33p462gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1mdeygb</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>I feel like they’re all a different shape</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdeygb</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1mdeo8a</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>My birthday is next week and I don’t know what to do to my nails… send help</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mdeo8a/my_birthday_is_next_week_and_i_dont_know_what_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1mdebq2</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Did Friend's Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7txzzkwx02gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1mddvxj</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Nail Glue Removal</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mddvxj/nail_glue_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1mddg2a</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Mooncat laquers are 🤌</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58qaedy0v1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1mddej2</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>if medieval nails are wrong, i don’t want to be right</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4q6uy3ou1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1mdd5aw</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Still trying to perfect builder gel!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uo62df52t1gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1mdd51d</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Void cat tribute nails</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdd51d</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1mdd3qp</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>My birthday nails!!! Jellyfish and bubbles 🪼🫧</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdd3qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1mdcz1x</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Semi-permanent nails with squares</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqm0h2lxr1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1mdcwps</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Growing out my nails help</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdcwps</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1mdcva4</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>My right hand nails come off every time</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mdcva4/my_right_hand_nails_come_off_every_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1mdcmdq</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Birthday nails for myself! Swipe to see them glow ✨️</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdcmdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1mdcmmu</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Summer yellow chrome Frenchies</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yflc3t3np1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1mdckzu</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>What shape??</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5b08rhcp1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1mdcesh</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>My favourite colour - Boston University Red. My nails have been so much healthier over the last year since I’ve been getting BIAB. What other colours would I suit to mix it up?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw812wo6o1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1md2bw0</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Would you put another set on these?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a3nh42zfzff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1md51wb</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>first time doing fake nails/press ons, any tips or tricks?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ja4gnqzf70gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1md0n8r</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Accidentally cut my nail bed with a knife</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9h4ch37xyff1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1md8hzq</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Got some ridges on 3 nails? Anyone else?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md8hzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1md7hc2</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>How do I Encourage my Nail Beds to Elongate?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1zn1e4hq0gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1md9qqo</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Fave sets since starting gel 1,5 year ago</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md9qqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1mdbxev</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Any fans of The Killers here?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdbxev</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1mdbwhg</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>New nails new me</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdbwhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1mdbtxi</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>2000s prom night style</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yb4why8dk1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1mdbrbn</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>How should I grow out my natural nails?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsp3uqmgj1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1mdbp75</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Space nails on myself</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wp3qasgj1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1mdbl0h</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Pretty Press Ons!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdbl0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1mdbi4y</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>First ever selfmade set!!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdbi4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1mdbdzy</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Recently started doing my own nails - advice?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdbdzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1mdaux1</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Mermaid Vibes. I tried a similar look and wanted to re-try.</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wapk8u5pd1gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1mdajz7</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Something Blue</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd83unrqb1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1mdabgl</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>UV glue recommendations please!!!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0ada5zp91gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1mda0w8</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>1st-4th attempt at gel x nails. Still clearly have ALOT of improvement to do. But I feel like I’ve made some progress since my first set 😅 open to tips and constructive criticism!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mda0w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1md9ozy</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Anyones nails look like this? :( I only paint them,(not fresh now though) nothing fancy but they look kinda bad with the weird lines. How to fix?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fp4ib0w51gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1md9ort</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Polygel for nails at Home</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1md9ort/polygel_for_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1mdvoxz</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Strengthening, base and top?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdvoxz/strengthening_base_and_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1mdu4aj</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Velma's vinyl bodysuit in the live action Scooby Doo 2 movie 🧡</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcztp372l5gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1mdtc1m</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Blurples!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3eram5oc5gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1mdqqqi</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>My friend said it looks like American Cheese 🤣</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51ix4cfbn4gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1mdq7xb</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Rosy red mani bc it's too hot</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lojlthtpi4gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1mdpuih</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Amber? More like honey!</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9bjhcppif4gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1mdpqad</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>SO RED</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdzxoegie4gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1mdpmb9</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Help with this effect, please!</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btcuhgi8d4gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1mdpcez</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>got distracted trying to feed the prince his dinner and now i’m in trouble</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdpcez</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1mdp2sl</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Dead House is GORG!</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdp2sl</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1mdo6ip</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>ISO a purple polish with gold or yellow or green shimmer/iridescence</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdo6ip/iso_a_purple_polish_with_gold_or_yellow_or_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1mdo3i4</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>To glitter or not to glitter? That is the question!</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x3l08cjl04gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1mdo21n</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Me: I need that Chameleon Nails shade. Also me:</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdo21n</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1mdj4pj</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>ILNP Pine &amp; Deep Space</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dbca2oc3y2gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1mdngog</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>my favorite "lighter" red polish!!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdngog</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1mdne28</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>like fire on my hands</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/modbmvvou3gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1mdmuts</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>First time nail art</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olb9oeq7q3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1mdmgjz</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>How do you create stripes with multicolored magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2q75kx1n3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1mdm0m0</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>DVN Flaming Hot Cheeto Dust</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdm0m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1mdlufh</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Starrily restocks?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdlufh/starrily_restocks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1mdlolx</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Which nail shape fits my hand the best??</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdlolx</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1mdkqjc</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>I damaged one of my nails, please help!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdkqjc/i_damaged_one_of_my_nails_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1mdk7su</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Kur Gel Shift Top Coat</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdk7su</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1mdjmmi</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Doomicorn</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdjmmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1mdj97b</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Does anyone know where to get these magnet stickers?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfuzfapxy2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1mdj8s1</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Tried magnetic polish for the first time</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d2fz1kvy2gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1mdj6gr</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Polishes that glow under blacklight?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdj6gr/polishes_that_glow_under_blacklight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1mdicii</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Offer advice to an aspiring Lacquerista please</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdicii</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1mdh4qo</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Best inexpensive efile?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdh4qo</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1mdgz7g</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Anybody heard of this brand? (UK)</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdgz7g/anybody_heard_of_this_brand_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1mdgwhx</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Distracting myself with shinies to not think about my PPU order</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/squcea5fi2gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1mdg3ud</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Wizard vibes ✨️</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdg3ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1mdfqzp</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>PSA for anyone seeking a one-coat wonder that makes nails look lit from within 🌟</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdfqzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1mdese8</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Talavera Nails 🦎🌞🍊🌊🍹</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdese8</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1mdeoje</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>One of my favourite summer manicures! August 2024</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btp5ncca32gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1mded32</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Decal fun!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yunqigu612gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1mdden3</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Are Yellow Polishes Automatically Prugly?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/km79ztz7g1gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1mdd9ya</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>What to do after injury?!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdd9ya/what_to_do_after_injury/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1mdcqg0</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Finally wearing my Polly Pocket polishes!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdcqg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1mdcjal</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Ninth (I mean Dead) House</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdcjal</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1mdcezk</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>"Professional" polish</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>/r/shortynails/comments/1mdaenq/professional_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1mdc7a2</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Heart &amp; Soul - Vanessa Molina, PPU July 2025</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdc7a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1mdb6le</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Favorite brand for sheer jellies?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdb6le/favorite_brand_for_sheer_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1mdb44i</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Magic Effect by DRK Nails- worth it?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdb44i</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1mdayx7</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Forgot I had this polish.</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qzw14xsie1gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1mdaxdr</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Summer time! Heat affects polish!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktz4yh88e1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1mdaasv</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Indie makers map? Affiliate code list/ sales list?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdaasv/indie_makers_map_affiliate_code_list_sales_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1mda7nk</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Grossest Polish Names?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mda7nk/grossest_polish_names/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1mda07j</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Bog Dweller with chrome 💚</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jnsqumj081gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1md9yw6</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Birefringence &amp; Jelly Fishing For Compliments</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md9yw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1md9lvt</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>PPU Order Came In!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1md9lvt/ppu_order_came_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1md9fjz</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>what do they mean by this 🧍‍♀️</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmnli50541gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1md949d</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Shower clean up hack</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1md949d/shower_clean_up_hack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1md90ba</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Tips for seche vite over designs?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dlx9wz711gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1md8dtz</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>It has come to my attention that I’m a dope…</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoek4cpvw0gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1md82gl</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Nail Polish Brands?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1md82gl/nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1md67v0</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Introduced mom to my world!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhqybbbxg0gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1md5w6j</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Why are there bumps in my polish?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md5w6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1md4ewu</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Last set before cutting down for work😭</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md4ewu</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1md3tpq</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Update: Redemption of the wrinkly nails!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md3tpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1md2g8n</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>PVB Free Base Coat</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1md2g8n/pvb_free_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1md1b8m</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Petty reasons you won't buy from a brand?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1md1b8m/petty_reasons_you_wont_buy_from_a_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1mduixt</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Rough draft of....</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbge29pnp5gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1md2kxp</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Hand-painted WEAPONS/Julia Garner Nail Art</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md2kxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1mdsvy9</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Katseye themed nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r33f0us085gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1mdsib7</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Summer Simple</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdsib7</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1mdshq9</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Tried my best at these clown nails I’ve been seeing</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdshq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1mdpwkw</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Acrylic jelly color tutorial</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5g11ua00g4gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1mdpoje</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Glossy Nails with Fuzzy Texture? The Contrast Is So Satisfying</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdpoje</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1mdoywo</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>DIY birthday set</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8jdrhq0484gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1mdn1m6</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>New nails, I loved them</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvlav9lrr3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1mdmxql</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>the least 3d set ive made in months</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ej242svq3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1mdlufj</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My first time trying porcellain nails, i'm going to add 3D lemons next</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdlufj</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1mdkuov</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Heart of the ocean</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddacqpoka3gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1mdjlhv</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Press On Nail Novice</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdjlhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1mdd1ff</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>First time blooming gel!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qiv7cmpcs1gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1mdcs28</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Nails made by me for my friend, how did they turn out?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdcs28</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1mdcb0s</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Void cat</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdcb0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1mdbz38</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>NYC Bratz Doll</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdbz38</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1mdavo5</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Mermaid Nails. Tried this look a while back but wanted to re-create again</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b5p846tud1gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1mdajbh</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Something Blue</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydgnu64mb1gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1md7cim</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Beachy Sets 🦪</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md7cim</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1md7bbl</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>I haven’t updated you guys in a bit!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md7bbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1md6vxq</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>I’m lowkey in love with them</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pug5yum2m0gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1md6bx5</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Orchid Nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awha4h3th0gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1md3snk</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Sharing my birthday nail! Swipe to see them glow ✨️</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md3snk</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1md3iqy</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Claws I made 😊</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oygeeyq9tzff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1md1tz6</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Some recent nails I made as a 17 yo beginner:)</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1md1tz6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug  1 08:14:10 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_03.xlsx
+++ b/data/collected_data/2025_08_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C915"/>
+  <dimension ref="A1:C1119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15988,6 +15988,3474 @@
         </is>
       </c>
     </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1mepy6y</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Before/After</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mepy6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1mepesj</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Finally got my nails done!</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mepesj</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1mepdqr</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>I have something to ask</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mepdqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1mep5vp</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Have a drink after getting nails down with my girl</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5yeudzfrcgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1meosnk</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>An attempt at my own nails 🤍</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meosnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1mek8up</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Kuromi Inspired Nails (OC)</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mek8up</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1menfxx</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>summer fruits!</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymmlens49cgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1memlyb</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Can I see everyone’s nailsss✨✨</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1memlyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1mem2d8</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Never going back</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mem2d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1melf8c</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>How much would you charge/pay?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwqg8m02qbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1meld4l</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>nails i got done yesterday</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfbfxtwfpbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1mel6om</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>summer</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mel6om</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1mekzsq</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>💃🏽🌶️</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa9f81mambgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1meksjs</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv8nukgikbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1mekshe</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Am I being too nitpicky? Paid $27 for just a gel color change</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mekshe</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1mekr2k</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Pretty in pink</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9eujso5kbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1mekdwk</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>I returned to the long 🫠</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mekdwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1mekaxr</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Opi Bubble Bath</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mekaxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1mejucb</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>How strong are BIAB nails actually?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mejucb/how_strong_are_biab_nails_actually/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1mejq22</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Ouch</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmcv3mw8bbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1mej83w</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>how much would you charge?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olz9sucz6bgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1meizqc</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>58 mins after my new set… rip thumb 😭</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ou80jatz4bgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1megh09</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>new base coat not working</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1megh09</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1meeaa4</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>My builder gel always peels off ONE particular nail and im not sure why</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meeaa4/my_builder_gel_always_peels_off_one_particular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1meg2d0</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>3D Lines Newbie!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onio5wc9hagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1mehonw</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Mix and match nails ✨</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mehonw</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1meiknu</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Medieval Court Jester-inspired Nail Art</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meiknu</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1mein5e</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>is my gel polish going to peel off?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mein5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1meiku3</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>First 3D set</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meiku3</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1meicn5</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Nail extension Refills</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meicn5/nail_extension_refills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1mei2r2</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Disney vacation nails done by me</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mei2r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1mehv24</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Refreshedddd💕</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mehv24</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1mehg3z</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>I Feel HAWWT 🥵🐆</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mehg3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1meh8r4</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Colour change for the upcoming semester (lecturer)</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmkcnf1kqagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1megwcx</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>For those that asked here is that update! First edition vs one year later! (Sorry posted wrong there first time)</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1megwcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1megtjo</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Pimped out my nail oil bottle to make obsessively applying it a little more fashionable</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8pcd5f6nagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1megs8z</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Nail Art Progress</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1megs8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1megs5d</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>First time getting nails done at a salon and idk if they're good</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1megs5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1meg5ie</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Went for a fun purple look this week.</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x806vh8yhagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1meg3b6</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>I can't stop looking at my nails🧙‍♀️🖤</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xcmu7xdghagf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1medfba</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Recovering nail biter</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1medfba/recovering_nail_biter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1mefnjb</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Blue chrome cat eye with some stars ✨</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mefnjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1mef1qm</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>I’ve wanted to get my nails done for so long!!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mef1qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1meel02</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Can I do that?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meel02/can_i_do_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1meejq2</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>(Continuation of my last post on this subreddit) Opinions on nail color?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meejq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1meeecw</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>A fresh nail art set 🐍☀️</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd39uwyx4agf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1medz6j</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>loving my vacation &amp; birthday nails!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9n9of4x1agf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1medywx</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>What do you think of my nails?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwdxam5v1agf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1medxei</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>What shape would look best for my nails?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnorvg1k1agf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1mecp9m</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Pink glass nails with chrome tips!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4pwn9o0t9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1mecni0</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>What do you think of my first baby boomers?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mddy87ees9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1mecifh</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7ibp8sor9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1mecgnf</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Some recent press on nails i have done 😁</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g0i8glcr9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1mecbsa</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>9d cat eye</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie70cc9fq9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1mec9hm</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Summer blues</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mec9hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1mec7r4</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Ruby armor nails</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu4rqycnp9gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1mebtwd</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Nails by me for my mermaid client 🤭🐚🦪</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5aewgd1n9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1mebe7a</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>my most perfect manicure !</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ihljjmxj9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1meb1ui</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Thick nail glue recommendations please?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meb1ui/thick_nail_glue_recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1meaus1</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>I loveeeee these nails my bf’s mom did for me ❤️❤️ I’m obsessed, I love herrr</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgoqktqbg9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1meb2f0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Las ultimas que me hice!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meb2f0/las_ultimas_que_me_hice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1meav71</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>soft chaos but sparkly this time</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnnd5fieg9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1meaqqm</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>How about this design today?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfugmk4kf9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1meaoie</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Bad French manicure</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meaoie</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1me9llk</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>I think this is my favorite mani I’ve made so far.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnhrof8t79gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1me9hze</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>New shape and first time venturing away from plain colour</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfzny3n479gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1me9ev9</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Funny lizard brain.</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/t/ZP8kUmdGK/</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1me5ox9</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Do these nails look well done?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7ovv6yfh8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1me61v6</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Why do my acrylics always lift 😭</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me61v6</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1me85s7</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Blue frenchie</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18xh67qzx8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1me85gi</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>The classic french fringe will never go out of style</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7qt6nqtx8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1me85fk</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>New mani, who dis?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ule6urrx8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1me8398</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>New set 🥰</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlr3jc3jx8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1me7xkd</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Your thoughts?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aj4mmbihw8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1me7lez</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>My nail tech put acrylic over this and said it was fine.</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xml27o29u8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1me7ia9</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>wedding nails?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1me7ia9/wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1me7876</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Nail strengtheners or hardeners that absorb</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1me7876/nail_strengtheners_or_hardeners_that_absorb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1me75vs</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Need advice for watercolor/ink nail art &gt;.&lt;</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me75vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1me704s</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Natural nails with pink armor nail gel</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me704s</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1me6k6e</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>I couldn't choose between the two, so I went for both!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8bamu7m8n8gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1me6hye</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Is this shady? I’m concerned about the (poly) in front of MMA instead of polymethyl</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oct9836um8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1me66p4</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Solid nail polish......yay or nay?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1me66p4/solid_nail_polishyay_or_nay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1me665r</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Sometimes when I see all the fancy nails on here I feel like I must be behind the times in nail fashion lol</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcxz1f4mk8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1me65bp</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Whats your favorite base color</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4ebjuock8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1me64qr</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Phantom of the opera set I did!</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me64qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1me5x2r</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>gel-x help</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me5x2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1me44sk</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Hygiene at nail salon</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1me44sk/hygiene_at_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1mdo2cl</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Nail bed massacre</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdo2cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1mdlf7y</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Burns?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdlf7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1mdni5u</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>What nail shape/length would suit me best?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdni5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1mdvxie</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>What is this dual form shape called?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdvxie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1mdskba</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Yellowish patch on nails?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6mr92xm45gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1mdya59</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>my bridal nails inspired by our wedding cake!! 🍰🍒</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdya59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1me5jyb</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Garden!</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrb995xig8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1me5h23</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Need help with prep and any other thoughts :)</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me5h23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1me58kx</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Lolla nails 🥳🩷🤭😍</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me58kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1me44sz</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Natural poly gel</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkv0d26x68gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1me3zic</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>First time getting my nails done 🤭</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/805qqk0x58gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1me3gil</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>First time getting acrylics for engagement nails!!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me3gil</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1me3eiq</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Made my second ever set of press ons, took me forever but i like them well enough!!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5hpgkfv18gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1meovdc</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>{PR} Just a little Augtober magic</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meovdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1meo2my</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>My July manis :) (more info in comments)</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meo2my</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1mengzv</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Pink Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/brhw3gvh9cgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1mem5r6</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>65lb circle magnet created an anti-bead effect??</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/40xty17xwbgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1mem2gd</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Experimenting with magnetic mix</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r86gnvi1wbgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1meljg6</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>What are your favorite highlighter yellow shades?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1meljg6/what_are_your_favorite_highlighter_yellow_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1melgmg</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Two coats funny bunny; one coat bubble bath OPI</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ts3etxaqbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1mel9n6</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>August PPU basecoat/topcoat questions</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mel9n6/august_ppu_basecoattopcoat_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1mel31d</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Just started my collection this year 😬</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mel31d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1mek512</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Ugh Idk if i’ve given myself contact dermatitis or if im being paranoid</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ppmdxiuebgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1mejrm0</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>i mixed this color :D</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjvl7tdmbbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1meiv2k</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Did I do it?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vpf955ev3bgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1meity1</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>THIS is the dopamine hit I needrd</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxr26h8m3bgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1meimgg</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>July Manis 🌞🍉🌳</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meimgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1meifq6</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Help me</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1meifq6/help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1meie7h</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Bkl Toil and trouble</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meie7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1mehyaj</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Royal Flame</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c0e9uj0awagf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1mehand</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>cornea killer 👁️👁️</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06q9cszyqagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1megvgx</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Mixing magnetics?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1megvgx/mixing_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1megitz</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My hands feel sticky after a manicure</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1megitz/my_hands_feel_sticky_after_a_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1megidf</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>DRK Magic Effect consistency</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s1tiqrepkagf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1megeg5</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>A new color every other day?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i0ispglvjagf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1mefydt</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Smoothing Base Coat Help</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mefydt/smoothing_base_coat_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1meexgz</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>4 Hours- Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcrt749q8agf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1meesu3</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Was going for Mermaid 🧜‍♀️ but I think I wound up with Fairy 🧚‍♂️</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxilnl1u7agf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1meeo2l</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Got my first build a gels :)</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meeo2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1meeko1</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Looking for top coat that won’t cause shrinkage on my nails?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1meeko1/looking_for_top_coat_that_wont_cause_shrinkage_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1medkab</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>First time using ILNP!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1medkab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1med985</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Gorgeous proto!✨</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1med985</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1mecyle</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>ISO darkish green nail polish with gold shimmer</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mecyle</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1mecji7</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>July Manis 🎆</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mecji7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1mebzva</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>💚 Polished For Days Quite Literally Dead Inside 💙</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mebzva</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1mebk16</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Anyone else worried about the new tariff changes?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mebk16/anyone_else_worried_about_the_new_tariff_changes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1mebiih</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>BKL Doomicorn 2.0 vs Polished For Days Lush</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mebiih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1meb6kb</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Shipping to Canada</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1meb6kb/shipping_to_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1meakvw</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Help me get over Purple Slushie</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1meakvw/help_me_get_over_purple_slushie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1me9rdo</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Please Show Me Your Battlestations!</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me9rdo/please_show_me_your_battlestations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1me9hzk</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>ILNP Sun-kissed</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/azpl03s479gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1me96kb</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>My Deco Beauty nail stickers are disintegrating????</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me96kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1me92ug</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Might be stuck at the car dealership…</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/upznypo749gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1me91p1</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>I polled my friends to rank my nail polish choices.</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://docs.google.com/presentation/d/1pUzolojKRzbTeUHsuHmnez69pQ6_VfbfpWxdshEsAbg/edit?usp=drivesdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1me8xwm</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>More nail stamping. Maybe I'll do all of them with this pattern.</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me8xwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1me8clv</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Stupid question - matte polish</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me8clv/stupid_question_matte_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1me868w</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Solar Polish + Sunscreen Questions</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me868w/solar_polish_sunscreen_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1me7o04</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Favorite Illuminator</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me7o04/favorite_illuminator/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1me75p7</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Tink’s Wings</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me75p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1me70lb</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>PPU Rewind</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me70lb/ppu_rewind/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1me6xtz</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>My perfect purple</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me6xtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1me6gon</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Whimsical manis</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me6gon</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1me6f2l</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>what i wore: july</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me6f2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1me4y5s</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Problem Resolution</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me4y5s/problem_resolution/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1me486t</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Playing with Mom's Makeup</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me486t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1me453n</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>cracked “ex-spearmint”🌿✨</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f8i4m1zy68gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1me40pj</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>First Fandom Flakies!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me40pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1me3xvd</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Roque Ocean Water</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me3xvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1me3p5b</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Dreamy Moonlit skies</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9z4r6btt38gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1me3hds</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>A good cuticle cutter and remover</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me3hds/a_good_cuticle_cutter_and_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1me34kq</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>More chipping with Nailtiques formula 2 as base coat.</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nx7ysdxz7gf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1me31nu</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Searching for this polish/similar shade</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpygpm6dz7gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1me2o33</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Bought it for the name but I am now smitten</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me2o33</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1me2ja7</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Did Holo Taco really just pull the Vacation collection to create FOMO??</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me2ja7/did_holo_taco_really_just_pull_the_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1me2ayp</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Oceanic Moonlight + Polar Lights 🌙⭐️</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me2ayp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1me1t31</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Happy ppu delivery day for me! This immediately went on both hands and toes 🦞</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me1t31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1mdja1s</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Am I being critical?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdja1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1me1eih</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>PPU Opens Tomorrow!! My wishlist is way too long and I feel like this month is almost better than July. What's everyone eyeing??</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc258tvin7gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1me18gw</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Lazy magnetic application success? ✨</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mnwjcaw7m7gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1me12rv</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Vacation Nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ar2ojlv0l7gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1me0rjx</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Need to franken something but don’t know the terminology - help?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1me0rjx/need_to_franken_something_but_dont_know_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1me0109</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Can anyone help me find a cat eye polish that matches this inspo pic</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2364b3pkc7gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1mdtfdf</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Pearly Pink Glazed Nails w/ Appliques</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yu90ke9nd5gf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1mdus5m</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Blueberry milk</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5inuubis5gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1mdyzqx</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Beginner advice</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mdyzqx/beginner_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1mdzdcd</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Help for peeling nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yswrykv67gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1mdxb0r</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Essie chipping easily??</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4s21le00m6gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1mdxau4</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Desperately searching for a dupe</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdxau4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1mdx3wu</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Orange Hot 🔥</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfmlpdbqj6gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1meqher</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>The Hidden NSFW Ones</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meqher</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1meov1y</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>am I insane for clashing hands?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6lwpa44ocgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1meotea</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>I did this just to try if I like the colors, I might do them cleaner. I really like them.</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meotea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1memgjr</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Snake skin nails. 🐍💅</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7xj0ymxrzbgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1mel5t3</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Porcelain Blue Nails.</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mm8zpopqnbgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1mehs1o</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Pink lemonade</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mehs1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1mehnew</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Mix and match nails✨</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mehnew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1mehju5</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>tried recreating nails i saw on pinterest</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x3an2j1tagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1meh266</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Summerween nails 👻💅</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meh266</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1megkse</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Has anyone tried translucent silicone brushes?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1megkse</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1megbcz</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>For those that asked here is that update! First edition vs one year later!</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1megbcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1mefeu5</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Obsessed with this set ✔️</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jpjief9cagf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1mef6hz</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Naturales con soft!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78orpdjgaagf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1mef376</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Gorillaz Nails</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mef376</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1mee7bh</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>isolated chrome is my passion.</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mee7bh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1mebrgf</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Practicing 3D fruits</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mebrgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1mebeql</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5s4pb75k9gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1me6yue</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Medieval Court Jester-inspired Nail Art</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me6yue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1me6shi</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Its LEO SZN bb🤩</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me6shi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1me5sut</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Mariposa</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5s6tfr5i8gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1me4ny0</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Tortoise Shell Nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me4ny0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1me384w</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>SMISKI NAILS</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgiz6lmm08gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1me2gh6</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Do you like these styles?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me2gh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1me144o</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Vacation mode ON🌴🥭🌺🌸</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me144o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1me0gf5</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>♡ .｡.:*☆ Exotic Colorful Flower Nails by Dew Doess Nails ☆*: .｡. ♡</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1me0gf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1mdyq5i</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>nail printing/ water decal</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mdyq5i/nail_printing_water_decal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1mdxmra</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>🫠🥹how’s it?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25w12zfkp6gf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1mdww49</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Limoncello</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mdww49</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug  2 08:11:53 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_03.xlsx
+++ b/data/collected_data/2025_08_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1119"/>
+  <dimension ref="A1:C1330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19456,6 +19456,3593 @@
         </is>
       </c>
     </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1mfl5b8</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>French on short nails</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfl5b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1mfl3tt</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>I love my new set</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9mrgwvpckgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1mfklcq</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Started doing my nails at home: here's the nail art I've done this far</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfklcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1mfkfgs</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Nurse wearing press ons</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfkfgs/nurse_wearing_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1mfkdff</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>silver glitter bc being chill is just not in my nature lately</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fe714v8c4kgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1mfk9h0</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>first time doing my own nails with gel!</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfk9h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1mfidqd</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Dark femme energy on my fingertips. 🖤</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vc60qhrrijgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1mfib6b</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>What specific non gel polish can I buy to match this?</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1pf5ax1ijgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1mfi9n9</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>New Shape</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h97tmpmhjgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1mfi1yj</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets my wife did recently!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfi1yj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1mfhl7h</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Are my nail beds more short or long ?😊</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rczwwbqvajgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1mfhbp9</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Cute little flowers</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efnwpnm88jgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1mfh3qa</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Fishy Fishies!</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adyuznr46jgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1mfgzdm</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Iconic French Tips</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxzpkz525jgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1mffre5</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>What do we all think about my ghost nails that I did ??</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mffre5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1mffqzd</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Neon stripes for summer</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shlvj8xltigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1mffn39</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>what does everyone think about infinite shine? this is my first one and idrk what to expect :)</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax9fzcglsigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1mffm4l</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>New Set 💕✨</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mffm4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1mffkoh</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Orchid</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjoxtzmzrigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1mfez7o</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Fruit nails inspired from a post in this group</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muwh6bgimigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1mfem7w</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Embracing my vampire era in the summer</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cvsnq0o9jigf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1mfehqg</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Summertime witchy vibes</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5dqjza5iigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1mfdjv1</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>What to do for a nail cracked at the base (under cuticle) after finger was deeply cut?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfdjv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1mfedbi</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Bootie.</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wqr4hv2higf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1mfe6yo</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>The end of an era</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfe6yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1mfdiwq</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>🍉 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k66x32i9igf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1mfdird</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Attempting butterfly wings!</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1v1c2wg9igf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1mfd1zx</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>My nail tech wanted to do sardines, who was I to argue? Probably one of my favorite sets she’s ever done.</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfd1zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1mfcupu</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Can’t do French tip pink base unless it’s gel??</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eskd8xll3igf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1mfcpyl</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Blue nails 🦋🪼🌊💦</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnlsvvag2igf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1mfcpab</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfcpab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1mfcowo</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>My wedding nails are atrocious</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfcowo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1mfcoo5</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I did my dad's nails</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfcoo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1mfc1sj</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Classic white nails</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pedx0euowhgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1mfbseq</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Sparkly ✨</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfbseq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1mfa637</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>First time getting acrylics and I got permanent white tips and my thumbs are in PAIN (can’t explain)</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzaqovzkhhgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1mf9ive</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Green for August 💚</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sxxgq9znchgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1mf96xl</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>PSA please do not put acrylic on your toenails</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mf96xl/psa_please_do_not_put_acrylic_on_your_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1mfbk25</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Nail extension refill</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfbk25/nail_extension_refill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1mfb7xv</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Today’s choice! My nail designer calls this “Maldives”</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03oh6vbvphgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1mfay30</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>When your new nails match your beverage 🥰</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kfgcm1onhgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1mfasdd</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>DND’s Fire Engine Red</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lk64ppwdmhgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1mfagyv</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Strawberry 🍓</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwn4gdqvjhgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1mfaghi</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Red Nails. That’s it. That’s the post.</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfaghi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1mfaewt</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Finally gave in and got “butter yellow” nails!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6amc03gjhgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1mfa8q9</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Questionnnnn</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68k047l5ihgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1mfa6pv</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Nail art!!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfa6pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1mf9cir</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>I love my nail tech 💅😍</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf9cir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1mf99xt</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>so so so so happy with this set</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf99xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1mf8v3b</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Ocean blues 💙✨️🌊</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8v3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1mf8ujp</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>French baliage</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz72rngm7hgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1mf8stz</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>I love minimalism</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcya6hn27hgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1mf8sqd</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Classy new set!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tut3xfu87hgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1mf8pki</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Porcelain Blue Nails. [Both Hands]</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8pki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1mf8g3l</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>First time getting cat eye!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8g3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1mf5y7g</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Hey everyone!!</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mf5y7g/hey_everyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1mf8521</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Black &amp; white, an iconic duo</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1o4ox3ci2hgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1mf7qa4</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf7qa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1mf7ocl</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Third set I've done on myself</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf7ocl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1mf7du1</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Getting ready for Halloween 👻</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf7du1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1mf7d2x</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>How to fix bendy natural nails whilst keeping gel on?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mf7d2x/how_to_fix_bendy_natural_nails_whilst_keeping_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1mf733o</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Muted color nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf733o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1mf72rx</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Chrome over cateye</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0rslvoqtuggf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1mf6nbp</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>I put a 3D charm on the underside of the nail. I love how it turned out 😇</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf6nbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1mf6cum</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Im in love with this color and shape</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjjgh62mpggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1mf6ay9</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>nail sets I’ve done as a beginner</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf6ay9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1mf69d9</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Tips, ideas?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgengvq1pggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1mf67cg</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>new nails 🪷</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyueq19boggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1mf61ie</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>I can't believe summer sets are leaving soon 😔</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf61ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1mf5dyc</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>What’s going on underneath my nails?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf5dyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1mf51wx</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Performer and Artist: Long wearing for lots of wear and tear</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mf51wx/performer_and_artist_long_wearing_for_lots_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1mf3er5</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Cat eye✨</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xd2f1sdj5ggf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1mf35bz</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>nails for my client 🌟</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf35bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1mf2zv7</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Do you prefer big or small nails?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47oz2b6r2ggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1mf29v4</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Gel polish allergy question</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mf29v4/gel_polish_allergy_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1mf2oix</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Second magnet gel attempt - Kokoist strawberry wine 🍓</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f5483sel0ggf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1mf2ghr</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Take me back to my vacation☀️🏝️🦩</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbyl6m03zfgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1mf20tt</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Akzentz Hybrid Pro 2.0 question on curing Luminary and DND</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mf20tt/akzentz_hybrid_pro_20_question_on_curing_luminary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1mesgj7</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Really really need help</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mesgj7/really_really_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1meq6if</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Sticky hands after a gel manicure</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meq6if/sticky_hands_after_a_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1mf1bif</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Matt design</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljftorafrfgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1mf0cuh</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Diy - pale lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf0cuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1mf07dw</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>🐱👁️</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf07dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1meza7a</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>The prettiest nails I've ever had done 😭 I'm in love</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meza7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1mez4ka</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>At home nails</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mez4ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1meykdf</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>I’m just a girrrl 🎀</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meykdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1mexy3r</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mexy3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1mexgnc</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Super fun dinosaur nails</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mexgnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1mexdeb</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Need advice/help pls</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mexdeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1mex9iw</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Well, I’m a short nail girlie now</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mex9iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1mex1vo</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Polkadot manicure!</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw6jem6wxegf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1mex0sr</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>I Love</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r5lxkr5nxegf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1mewxia</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Vampy nails part 2</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mewxia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1mewxa4</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Just look at these😍</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mewxa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1mevgz3</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Would it be possible?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mevgz3/would_it_be_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1meuyy1</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Gel, acrylic, or natural</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1meuyy1/gel_acrylic_or_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1meufs2</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Neon French tips</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01vqy0dwcegf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1mesrf7</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>First time with cat eye!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuynil1bwdgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1mesc3h</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Pink chrome 💅</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gl29aw1urdgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1mes89z</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>I have no words. I haven’t broken a nail since may.</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mes89z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1mfko3h</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Mooncat Epilogue To Utopia</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfko3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1mfjzi5</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>in love with this green 💚</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfjzi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1mfjpu5</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Glass bead without the horseshoe magnet?? It's possible!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yxezmnjzwjgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1mfjpa6</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Mesmerised!</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo9bzp21xjgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1mfjlk0</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Oldie but goodie…</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfjlk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1mfjcgp</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>HELP!! This Brazilian polish is way too cute😭</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9ujeqmvsjgf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1mfj65s</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I Exaggerate Absolutely Nothing Ever</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mcs72sf4rjgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1mfiv21</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Do I want the impossible? Alternative to builder gel</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfiv21/do_i_want_the_impossible_alternative_to_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1mfiuam</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Sabrina Carpenter on Stephen Colbert a few months ago. jelly lilac pink. 😻can anybody id?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3zgqzelnjgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1mfgl90</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>First time trying nail art</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i2z3x8e1jgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1mfg02k</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>I love greeeeens</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvnxon4xvigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1mextjh</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>How do I make my nails last?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgps3u8i2fgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1mf07m2</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>New Brand Introduction - Aura Bloom Polish</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf07m2/new_brand_introduction_aura_bloom_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1mffns1</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Fun with magnets and glitter</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/st7naddrsigf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1mfffvc</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>KBShimmer vs Rogue Lacquer Flakies</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfffvc/kbshimmer_vs_rogue_lacquer_flakies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1mffdxh</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Are my nails too over filed for acrylic? I just took dip off, my nails are sensitive and I want to acrylic to cover them.</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mffdxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1mfea8h</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>qipao nails</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfea8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1mfe9l6</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>VIP by ILNP - Magnetized</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/83zucch5gigf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1mfe54z</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Flaking nails :(</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfe54z/flaking_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1mfdqvq</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Jinx x Rapunzel Mani 💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfdqvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1mfdp8m</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Where my goblin queen laqueristas at?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dz612u2bigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1mfd8o2</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Peridon't bother me</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4j66ipfs6igf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1mfd3jk</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Glitter Experiment!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mza7f85w4igf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1mfcgbe</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Help me find this vintage bridal OPI from 2000?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfcgbe/help_me_find_this_vintage_bridal_opi_from_2000/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1mfc6om</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Am I the only one who likes the look of dispersed magnetics?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfc6om</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1mfc6e3</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>St. Tropez Fading?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfc6e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1mfbzm2</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Aurora Beam</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfbzm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1mfbyad</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Precious Cargo</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/di1fjczdvhgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1mfbnv3</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Growth and Decay</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfbnv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1mfbhsj</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Birthday Weekend Mani</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfbhsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1mfaoyj</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>on the prowl…</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfaoyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1mf9iz7</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Swamp Gloss "Swift and Saddled" - solar + glow in the dark! ☀️</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wvo5c3pchgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1mf9gia</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Green for August 💚</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9m9p92q5chgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1mf9fo7</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Plum/Burgundy with aqua shimmer</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf9fo7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1mf9bge</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Tried out the flower trend</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf9bge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1mf9alu</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>The only unidentified shade in my collection</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf9alu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1mf8wza</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>I joined the Moonies (Mooncat newbie here).</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8wza</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1mf8u5n</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>I’m very new to nail polish. What is going wrong?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yaqh0wj7hgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1mf8p1i</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Cleaning</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf8p1i/cleaning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1mf8ivu</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Pangea in a bottle</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8ivu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1mf8cho</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>My first mani post-op!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8cho</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1mf8b3n</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Leelanau Auroras - 1422 Designs (PPU Rewind)</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc340tqp3hgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1mf8anh</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>absolutely mesmerised 🤩</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf8anh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1mf7yz0</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Cuticle help</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf7yz0/cuticle_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1mf7yaz</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Magnetic pigment scratches an itch in my brain</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3f8ihcn51hgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1mf7ukw</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>PSA: Tariffs🍁</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf7ukw/psa_tariffs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1mf7rco</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>vine nail art with regular lacquer?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf7rco/vine_nail_art_with_regular_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1mf7j2b</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>She really is that girl ✨</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf7j2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1mf6z01</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Clionadh "Still no Pickles!" and Embellishment</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf6z01</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1mf6tqm</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Pearly opaque nail color for bride? (Show your wedding nails!!)</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf6tqm/pearly_opaque_nail_color_for_bride_show_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1mf6m36</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Vitamin E for splitting nails?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ca2t8mbkrggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1mf6gh7</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Lemon, Meet Your Sibling</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/msy8p2ufqggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1mf64n6</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Summer Favs ☀️</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf64n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1mf63cu</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Sally Hansen | The Queens Velvet</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utzk1qmenggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1mf63a5</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Cuticula - Dead House + cat tax</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf63a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1mf60x3</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Deciding It's Worth It - BKL</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h4l9u9enggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1mf5l2s</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer Bog Dweller Bead Style</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8lq1sha4kggf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1mf5i5o</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Did I dupe Lahar?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nthgsg5qjggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1mf57qe</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Clapping to you people</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf57qe/clapping_to_you_people/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1mf4t0e</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>My Thrifted Haul</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf4t0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1mf4n2q</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Experimental Marsala Jelly toppers</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14zm5l4tdggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1mf48l3</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>2 Weeks</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf48l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1mf45g2</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Summery Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf45g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1mf41ep</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Found a use for SuperNail Thinner the no-no product</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf41ep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1mf417c</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Liquid Sand</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf417c/liquid_sand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1mf411t</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Help Identifying an Essie Polish Color</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf411t/help_identifying_an_essie_polish_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1mf3o3t</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Ruby throated dupe?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uadmle497ggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1mf33xb</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>The demon screech I let out when I opened my mail box this morning 👹</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5ua053j3ggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1mf33kh</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Dead But Delicious</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf33kh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1mf30z7</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Beaux Rêves - Ghost Ship</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf30z7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1mf2m1b</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Butterfly Wings</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf2m1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1mf2ln6</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>first time layering these!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdty9z620ggf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1mf26dl</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>an update on my absolutely unhinged spinning magnet</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6hb0ul18xfgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1mf1gz8</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Obsessed with velvet magnetics recently—same polish, slightly different angles!</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtwsrnehsfgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1mf1dys</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>How do you organize your polish collection?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf1dys/how_do_you_organize_your_polish_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1mf1738</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Love to Love You🩵✨</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf1738</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1mf0wcf</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Why do some American brands charge tariffs but not others?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mf0wcf/why_do_some_american_brands_charge_tariffs_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1mf0r1a</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Dead House by Cuticula</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a1cgnbjnfgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1mf0kr5</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Painting over nail-nail bed separation? (No infection)</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nzgbdfcmfgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1mf0c1a</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>It’s giving wicked step mother</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jty6z7ftkfgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1mf01af</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Perfect for the August heat 💚</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lul9gfuqifgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1mezrmb</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Tried the glass bead method!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g6nf3sktgfgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1mezr9j</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Pink with Purple Shimmer or Purple with Pink Shimmer?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mezr9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1meznf3</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>What's your favourite beetle green?</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n3kqld4gfgf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1mezmer</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Lurid lacquer swatch request!💚</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uarue5lvffgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1meyxvg</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Stickers lifting</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meyxvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1meyqor</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Tomato, Tomahto</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u5sd5fz9fgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1meyobp</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Nail Illuminators/ Concealers</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meyobp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1meym17</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Blue for a rainy Friday ☔️</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlxunfv19fgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1mey6n2</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 Plus</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mey6n2/nailtiques_formula_2_plus/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1mextav</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Lavender nail art</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mextav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1mexk93</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Still summer</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97u080zk1fgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1mexe1k</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>4th mani of the week 🤦🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgbj8o8c0fgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1mex3w5</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Getting much more confident with application technique!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mex3w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1mewvlo</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Can't Find Nailtiques Formula Fix Thinner</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mewvlo/cant_find_nailtiques_formula_fix_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1mewva7</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Okay Baroness X!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mewva7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1meweud</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>First sassy sauce purchase 💕</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s7t0po3tegf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1mew1j8</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>🐈‍⬛ Cat Approved</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mew1j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1metjkv</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Essie Cap Snapped</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a4hqafe4egf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1mesg0u</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mesg0u/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1mfkyhz</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Homemade Brass fingernail</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0j2p8c0bkgf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1mfjq1y</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>3D fruit press on set</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcab3cg9xjgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1mfi4zt</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Nail art!</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kn2bepcgjgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1mfh3sa</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Was Really Proud of How These Turned Out for my Client!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfh3sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1mfh2ho</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Chinese watercolor painting</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bt8ihpt95jgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1mfgq3q</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Ring stack set ✨</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r65we4ol2jgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1mffsza</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Simplicity speaks volumes. 💅✨</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egox74k4uigf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1mfddqr</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Toile Du Jour nail stamping practice set comparing different opacity, luminosity and contrast options</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ztgbbpb58igf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1mf49kj</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Metalcore fire heart nails</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf49kj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1mf06iv</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>just want to show these off 😘</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mf06iv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1meyx25</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Mixed-inspo DIY nails</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1meyx25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Aug  3 08:11:55 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_03.xlsx
+++ b/data/collected_data/2025_08_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1330"/>
+  <dimension ref="A1:C1530"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23043,6 +23043,3406 @@
         </is>
       </c>
     </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1mgdte2</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Didn’t bedazzle my whole hand this time. Progress?</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vdtgzteirgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1mgdajp</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Ask me anything about nail tools.</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mgdajp/ask_me_anything_about_nail_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1mgd6xh</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>First time getting nails done, is this normal?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mgd6xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1mgco3l</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mgco3l/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1mgci52</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>First time doing a character nail!</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mgci52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1mgbvd2</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>What are the sticks called?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3yp5w73wqgf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1mgabp3</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Nail keeps breaking despite everything I've tried</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyo2nxtxfqgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1mg9pp0</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Sticky tab preparation</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mg9pp0/sticky_tab_preparation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1mg8hwf</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Wedding nails dilemma!</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mg8hwf/wedding_nails_dilemma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1mg7xht</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>ombre 💙🤍 BIAB</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg7xht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1mg8czj</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Looking for a translucent purple gel polish that looks like this!!!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yk1d5y0xpgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1mg74ew</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>HELP! am i cooked😭</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg74ew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1mg77m3</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in an attempt to thwart my nervous picking habit and omg 🥺🧡</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh1l9zjhmpgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1mg70vk</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>New nails 🌷🐦‍🔥🪷</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg70vk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1mg6vqk</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Press ons..</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg6vqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1mg6jrh</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Money green please 😊</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8036oifgpgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1mg6iyd</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Enjoying my pregnancy nails while they last! 🤍</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg6iyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1mg5yw3</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Does it still count if it's stickers?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg5yw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1mg64nf</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>What’s going on with my nail?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx45mdblcpgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1mg6gs1</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Nail Day</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj3wiybafpgf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1mg6g5k</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Nail set my brother made for me! 🦇</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg6g5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1mg6djd</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Italy Nails</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg6djd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1mg66c4</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>My latest fill 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg66c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1mg641q</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Ms. Mooncat Fake Halo saving me from catastrophe</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgg3bhrfcpgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1mg5u5x</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>New Set ❤️</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvdvvuqy9pgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1mg5mbc</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Am I doing this right?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg43sll08pgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1mg4axc</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Sore fingers after uv gel</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mg4axc/sore_fingers_after_uv_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1mg4ite</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Did I mess up taking off my gel polish?</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8go49jnhyogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1mg4jju</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>I was going for a y2k emo vibe</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg4jju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1mg5cas</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>I think they’re cute 🥰</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swv3v3il5pgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1mg5b8v</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Sin dudas esta hermoso o no?</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg5b8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1mg59ty</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>🍋 lemon nails</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j87vs9lz4pgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1mg595a</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>natural nails with gel overlay 💖✨</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg595a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1mg54oi</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Catch of the day nails</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg54oi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1mg50rc</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Cute lil set I made for my vacation 🖤</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygijfvys2pgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1mg4nbf</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Strawberry matcha inspired nail set</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6nsdz9wizogf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1mg4hbu</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65ki34a5yogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1mg4bec</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Minimalist Sparkly Nails</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg4bec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1mg48fn</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Just a simple little something! Only took 3ish hours!</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izec6cy1wogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1mg3x7z</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Finally proud to show them off</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi9oro3gtogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1mg36wc</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Black Pink Nail Design</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg36wc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1mg34p8</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Faerie rings</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg34p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1mg341o</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>First time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jv6dd9rmogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1mfyzyb</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Can anyone tell me how to fix my jank nails</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfyzyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1mg125s</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Polygel comes of without damage to the natural nail</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mg125s/polygel_comes_of_without_damage_to_the_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1mg2o2s</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Beginning of August means Halloween Nails (basically)</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg2o2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1mg2kif</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>wicked mani</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg2kif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1mg2f8f</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Obsessed with my Nails</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg2f8f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1mg24qp</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Got gel x for the first time. Should there be this much gel underneath the thumb? Do I go back and ask them to drill it down?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg24qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1mg1dsi</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Help me understand</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mg1dsi/help_me_understand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1mg1e2x</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Super cute color (yes, this is orange), I did it by myself</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2h8mc749ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1mg144n</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>August nails</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icw688cx6ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1mg0aii</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>First time trying long drawing brushes.</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y649o5ul0ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1mg0a8e</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>In love with this color! *Feet in 3rd pic*</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg0a8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1mg04i3</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>My perfect red 🖤</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abz1xflazngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1mfzt25</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Really liking this color</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfzt25</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1mfy78h</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Fix nail or new set?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vm68q5kkngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1mfyvkd</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Gel nail fill procedure??</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfyvkd/gel_nail_fill_procedure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1mfziv8</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Obsessed with my ocean inspired nails!!</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfziv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1mfznhd</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Biab split nail suggestions</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgoeohjnvngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1mfzmg4</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Amazon Press Ons</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yvt3ugevngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1mfzm13</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Delicate nails</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcxn15mbvngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1mfz2dq</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Can I blow dry my hair with acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfz2dq/can_i_blow_dry_my_hair_with_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1mfyt5o</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Concert nails</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo3277k6pngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1mfyt49</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Rawr</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zetssrk5pngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1mfyrtq</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>My claws today!</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e7vzu3wongf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1mfyr8s</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>My girlfriend is a nail tech and she did her own nails, she's too shy to post but I thought its worth sharing</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2vptyzrongf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1mfycsc</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Cateye &amp; Flowers ☀️</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn0hnuvplngf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1mfyboj</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>What gel polishes work with an LED lamp?</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgo1m6rhlngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1mfy1o3</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Does anyone have a good equivalent of OPI’s “Put it in Neutral” that’s a darker brown?</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yh041fdjngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1mfy0wp</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>My cuticles are look like this after a couple weeks… help!</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfkkfs97jngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1mfy0v5</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>My wedding nails are no longer atrocious (but that salon is)!! Update</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfy0v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1mfxyiw</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Summer neon ☀️🍉</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk7tdznoingf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1mfxg2i</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>If you put gel on your own press-ons, don't sleep on magnetic nail stands right on the metal bottom of your curing light!</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfxg2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1mfxbd2</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfxbd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1mfx5hy</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Press ons lasting longer</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfx5hy/press_ons_lasting_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1mfwnek</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Finding a good nail tech is hard</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfwnek/finding_a_good_nail_tech_is_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1mfx4jf</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>My nails for august, is it good?</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6igb99jecngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1mfwzh2</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Loving my nails for Lady Gaga’s Mayhem Ball. Paws up, Little Monsters!</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20gkuy7dbngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1mfwuxh</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Two hours of work..</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfwuxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1mfwi2p</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Does rubber top coat work? Any recommendation?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfwi2p/does_rubber_top_coat_work_any_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1mfwbbi</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Suggestions on nail shape? Getting a full set in a few hours and it’s been a while!</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfwbbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1mfw6gl</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Ponyo press-ons 🪼</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfw6gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1mfw04l</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Summer Nails!</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ahmo6o24ngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1mfvmvu</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Some of my favourite sets</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfvmvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1mfvmxx</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Spoiler for jump scare</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfvmxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1mff8z5</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Why do I have so many cuticles?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mff8z5/why_do_i_have_so_many_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1mftl39</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Break up with nail lady?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mftl39/break_up_with_nail_lady/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1mfqzqf</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24c4vnta2mgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1mfq5ys</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Eye allergy to nail polish</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfq5ys/eye_allergy_to_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1mfq4m3</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Unsure if gel is cured?</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfq4m3/unsure_if_gel_is_cured/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1mfpzqc</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Something weird is happening to cuticles</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfpzqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1mfv4na</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Pinks</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfv4na</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1mfgeiw</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Would you recommend this nail kit for beginners?</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://a.co/d/eL1yMdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1mfk9t3</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>2-in-1 perform better as base or top coat?</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mfk9t3/2in1_perform_better_as_base_or_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1mfkm18</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Do these suck or have I just gone too long without nails</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfkm18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1mfv0xh</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>We have claws to show off 🐾💅</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbcufebrwmgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1mfs96o</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>The most beautiful hand-painted nails ever!!</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfs96o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1mfuupp</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Nails for one of the fav months😻</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfuupp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1mfueki</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Aphrodite’s nightie by opi</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgco7vb3smgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1mgd9qi</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Do you feel happy when your polish shows a fill line?</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywu6hvp0crgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1mgcsh7</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>First EVER black nails</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mgcsh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1mgcnjy</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Mooncat Gradient ☔️</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mgcnjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1mg9sqs</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Choose your all time fave</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg9sqs/choose_your_all_time_fave/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1mg9npy</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Canadian Peel off base coats?</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg9npy/canadian_peel_off_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1mg9dy7</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Troubleshooting mani issues (chipping / lack of longevity)</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg9dy7/troubleshooting_mani_issues_chipping_lack_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1mg8oxy</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Orange glitter mix</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg8oxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1mg838a</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Had to stop mid mani to admire this</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8eswahoiupgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1mg7krw</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Psylocybin 🍄</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/10tef0loppgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1mg7hf6</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Love this color!</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82lmbxiyopgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1mg7aub</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>Highlighter bright</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg7aub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1mg6htc</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer Prototype X11</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg6h3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1mg69sh</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Cottagecore</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg69sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1mg5qzn</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>How do I make cleaner stamps?</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg5qzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1mg5ken</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Any gamers gotten polish on their laptop? 😅 Tips for removal?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg5ken/any_gamers_gotten_polish_on_their_laptop_tips_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1mg55xn</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>User error or top coat issue?</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg55xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1mg4ys3</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Baroness X Acetone Antidote is Witchcraft</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzg0jk9b2pgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1mg4nim</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Recommendations for good cruelty free + vegan cuticle remover?</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg4nim/recommendations_for_good_cruelty_free_vegan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1mg4h9x</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Very impressed!</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg4h9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1mg46jf</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>You Are A Wonder 😍</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7oa8kk1lvogf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1mg40v2</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>First thermal</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg40v2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1mg3ruh</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>It was nail day at our house today! I always get the best requests from my daughters 😆</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg3ruh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1mg36j6</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Backlight mani</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55wg9id0nogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1mg34td</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>What non-cremes resemble Big Apple Red by OPI?</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg34td/what_noncremes_resemble_big_apple_red_by_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1mg31cg</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Vibes of late summer with a hint of fall 🍃🌞</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rf4xv1yvlogf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1mg2wly</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Kabernet Kisses</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg2wly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1mg2pnh</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>You long-nailed laqueristas are heroes 🫡 it takes so much polish for this...</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c7d94ygjogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1mg29nr</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>How to get better longevity out of linear holos</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrxmwirsfogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1mg26jn</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>ILNP's Amber is brilliant</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg26jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1mg1xvb</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>ILNP Rosewater ✨💎</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg1xvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1mg1xao</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Indecisive swatch day + a very forgiving, gloppy black</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg1xao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1mg1odu</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>2 Months in another country. What nail polish to bring?</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg1odu/2_months_in_another_country_what_nail_polish_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1mg1hqv</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Found at Big Lots! $2 or less per bottle</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg1hqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1mg1cmo</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Random request! Skinny rectangular empty bottles?</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gbb1gjs8ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1mg1afk</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Permanent vertical split in my nail - any advice?</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fti6q8b8ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1mg15pf</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Your recommendation of 'girly' gel Polish for 18 year old niece?</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mg15pf/your_recommendation_of_girly_gel_polish_for_18/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1mg10oz</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>How do you make a regular sheer polish look more plump? I add two coats of thick top coat but it’s not enough.</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/uWt1n1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1mg0yo1</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>it's been a while since i used nail polish so ...</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg0yo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1mg0uwf</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Sometimes you just need your favorite red ❤️</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg0uwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1mg0mne</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer This Comfort Now Constrains You</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eker6p63ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1mg0c8w</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>First time..</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x253pn7z0ogf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1mg0a5r</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Halo Taco | Toe Beans</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq0vby9e0ogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1mg03ri</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>BKL mosaic magnetics 🥰</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j1ykq1v4zngf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1mfyagb</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>I did it! Butterfly art 🦋</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud6yvlh8lngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1mfy14n</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>I live in MN so I had to visit!</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7gs9449jngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1mfxdhc</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>How long do the vibrant scents products’ scents last? Is it until they dry down, days, weeks…?</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfxdhc/how_long_do_the_vibrant_scents_products_scents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1mfx4a9</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Ughhhh, wtf...</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0t3xhpccngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1mfwvpt</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>What's your nails kryptonite?</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfwvpt/whats_your_nails_kryptonite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1mfwh1v</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Question</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfwh1v/dazzle_dry_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1mfw0bv</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Y’all…this might be my favorite mani so far!🔮✨</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfw0bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1mfvmz6</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Perfect lighting 🌈</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdtx16ra1ngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1mfv29g</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Blood red polish</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xouwjo0xmgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1mfuwdy</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Castor✨🪐</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/joieoyrrvmgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1mful8g</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>First indie polish</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mful8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1mfu2ef</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Easiest magnetics/cat eye polishes to work with?</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfu2ef/easiest_magneticscat_eye_polishes_to_work_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1mfu1bn</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>✨️💙Band Camp Sparkle Bomb🩵✨️</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfu1bn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1mftm08</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Cross Velvet? Style “My Life as a Shrimp”</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mftm08</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1mftbai</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Saturday manicure</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mftbai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1mfstb1</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>Faerie Rings</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfstb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1mfsqhm</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Cadillacquer’s Orchid</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfsqhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1mfsqe9</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Latest mani with cat tax</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfsqe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1mfsmvv</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>House of Hades Dupe?</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfsmvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1mfs7s6</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Revlon Top Speed Blues</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iphxb5pubmgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1mfs6nb</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Revlon - Bottle Top Styles</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfs6nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1mfs62k</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Essie “Style Hunter” dupe?!</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfs62k/essie_style_hunter_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1mfrx83</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Second at home nail set - how did I do? Is there something to be improved?</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wczi024p9mgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1mfrvh0</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>This time I made this design and I liked it a lot.</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as7vlh7b9mgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1mfrfgw</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Mooncat Aphrodisiac</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfrfgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1mfr4ka</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>ILNP Snowstorm</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfr4ka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1mfqjdo</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Inspired by my cats</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfqjdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1mfq9ju</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Organization advice</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me760sy7wlgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1mfq29z</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Customer Service</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mfq29z/death_valley_nails_customer_service/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1mfpw90</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Cosmic polish - hidden depths</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0k2t4k0tlgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1mfpnzh</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>Tried Some Jelly and Holo</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfpnzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1mfph9a</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>Who else is ready for Halloween in August?</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfph9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1mfp1xr</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Is this considered a glass bead finish?</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4quwjvm9llgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1mfn6l1</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Mooncat, u outdid it</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ssjhq5jh1lgf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1mflrra</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>First time Cat Eye</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mflrra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1mflkdx</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>How do I purchase By Vanessa Molina???????</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mflkdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1mg6ln0</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>What do you think of French?</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8drb0puwgpgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1mg6i8o</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Italy vacation nails</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg6i8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1mg4cjk</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>Been getting a lot of green orders in ✨</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rmk0hxkzwogf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1mg46vc</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Just a simple little something today! Only took 3-ish hours.</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7bv2vkovogf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1mg3rfc</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Teef</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg3rfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1mg2be2</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>Which picture looks best for these nails????</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg2be2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1mg24m0</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>This is the first time I've done my own nails, something simple but it's my triumph.</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mg24m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1mfzjxs</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>Talk to me about love for nails 😍 What do you think of the design I made today?</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfzjxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1mfyn3z</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Little fishy</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6hz2b7wnngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1mfy3df</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Clown/circus set</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6z6vzrqjngf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1mfy26t</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Why is the polish changing from purple to gray. These are my moms nails that I did. Both pictures are of her nails. I am a tech who will be receiving license soon. Went to empire beauty.  Sorry for the repost, the other one was removed.</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfy26t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1mfxfea</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Did my friend’s nails!</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfxfea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>1mfx0gv</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>My new summer fruit nails 🍊🍋🍒🍓🥝</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfx0gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>1mfwzer</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Nail stamping plate cleaning advice</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwxnm03yangf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>1mfwczp</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>NEED YOUR HELP!! My uni having an art and craft expo sell and I decided to sell a few nail set, I need to know if am missing any themes, aesthetic or vibe!! (Details below)</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfwczp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>1mfw8q2</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Ponyo press-ons 🪼</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mfw8q2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>1mftn6o</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>Safe way for kids to do nail art</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mftn6o/safe_way_for_kids_to_do_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>1mfslnm</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>Rockin’ the Croc hands</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9e7bj5temgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>1mfrtp3</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>Second at home nail set - how did I do? 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psal7tmw8mgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>1mfprvm</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>ILNP Amber may be the perfect honey polish 🐝🍯</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4appcnwwrlgf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>1mflvgo</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>Ohh, I'm loving this design that I did..</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DM1UX9bOgAv/?igsh=MWoycTBmenZ5bmY5cQ==</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>